<commit_message>
Fix case loading issues.
</commit_message>
<xml_diff>
--- a/Cases/Cases1.xlsx
+++ b/Cases/Cases1.xlsx
@@ -1,38 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28502"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jia/Dropbox/v2test/Cases/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17620"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Tests1" sheetId="1" r:id="rId1"/>
-    <sheet name="Tests2" sheetId="2" r:id="rId2"/>
+    <sheet name="Tests1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Tests2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tests1!$A$1:$K$41</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
   </definedNames>
-  <calcPr calcId="0" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="130">
   <si>
     <t>Run</t>
   </si>
@@ -67,114 +69,117 @@
     <t>Failure Message</t>
   </si>
   <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>AT.UI.Home.01</t>
+  </si>
+  <si>
+    <t>Home(Default URL)</t>
+  </si>
+  <si>
+    <t>Default URL</t>
+  </si>
+  <si>
+    <t>ui</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>2017-09-28 21:57:17</t>
+  </si>
+  <si>
+    <t>AT.UI.Home.02</t>
+  </si>
+  <si>
+    <t>Home(Custom URL)</t>
+  </si>
+  <si>
+    <t>Custom URL</t>
+  </si>
+  <si>
+    <t>http://www.baidu.com</t>
+  </si>
+  <si>
+    <t>2017-09-28 21:57:20</t>
+  </si>
+  <si>
+    <t>close</t>
+  </si>
+  <si>
+    <t>http://www.bing.com</t>
+  </si>
+  <si>
+    <t>AT.UI.Search.01</t>
+  </si>
+  <si>
+    <t>Search(Save element)</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>2017-09-28 21:57:25</t>
+  </si>
+  <si>
+    <t>Search box</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>kw</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>(Save element)</t>
+  </si>
+  <si>
+    <t>save</t>
+  </si>
+  <si>
+    <t>searchbox</t>
+  </si>
+  <si>
+    <t>Search btn</t>
+  </si>
+  <si>
+    <t>su</t>
+  </si>
+  <si>
+    <t>click</t>
+  </si>
+  <si>
+    <t>AT.UI.Search.02</t>
+  </si>
+  <si>
+    <t>Search(Load the saved)</t>
+  </si>
+  <si>
+    <t>2017-09-28 21:57:32</t>
+  </si>
+  <si>
+    <t>(Load the saved)</t>
+  </si>
+  <si>
+    <t>saved</t>
+  </si>
+  <si>
+    <t>wait</t>
+  </si>
+  <si>
     <t>n</t>
   </si>
   <si>
-    <t>AT.UI.Home.01</t>
-  </si>
-  <si>
-    <t>Home(Default URL)</t>
-  </si>
-  <si>
-    <t>Default URL</t>
-  </si>
-  <si>
-    <t>ui</t>
-  </si>
-  <si>
-    <t>open</t>
-  </si>
-  <si>
-    <t>pass</t>
-  </si>
-  <si>
-    <t>2017-09-28 19:01:40</t>
-  </si>
-  <si>
-    <t>AT.UI.Home.02</t>
-  </si>
-  <si>
-    <t>Home(Custom URL)</t>
-  </si>
-  <si>
-    <t>Custom URL</t>
-  </si>
-  <si>
-    <t>http://www.baidu.com</t>
-  </si>
-  <si>
-    <t>2017-09-28 19:01:43</t>
-  </si>
-  <si>
-    <t>close</t>
-  </si>
-  <si>
-    <t>http://www.bing.com</t>
-  </si>
-  <si>
-    <t>AT.UI.Search.01</t>
-  </si>
-  <si>
-    <t>Search(Save element)</t>
-  </si>
-  <si>
-    <t>Search</t>
-  </si>
-  <si>
-    <t>2017-09-28 19:01:47</t>
-  </si>
-  <si>
-    <t>Search box</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>kw</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>(Save element)</t>
-  </si>
-  <si>
-    <t>save</t>
-  </si>
-  <si>
-    <t>searchbox</t>
-  </si>
-  <si>
-    <t>Search btn</t>
-  </si>
-  <si>
-    <t>su</t>
-  </si>
-  <si>
-    <t>click</t>
-  </si>
-  <si>
-    <t>AT.UI.Search.02</t>
-  </si>
-  <si>
-    <t>Search(Load the saved)</t>
-  </si>
-  <si>
-    <t>2017-09-27 17:53:14</t>
-  </si>
-  <si>
-    <t>(Load the saved)</t>
-  </si>
-  <si>
-    <t>saved</t>
-  </si>
-  <si>
-    <t>wait</t>
-  </si>
-  <si>
     <t>AT.UI.Login.01</t>
   </si>
   <si>
@@ -307,9 +312,6 @@
     <t>jiangjia</t>
   </si>
   <si>
-    <t>y</t>
-  </si>
-  <si>
     <t>AT.HTTP.Get.01</t>
   </si>
   <si>
@@ -325,7 +327,7 @@
     <t>https://github.com/timeline.json</t>
   </si>
   <si>
-    <t>2017-09-28 19:40:14</t>
+    <t>2017-09-28 21:57:36</t>
   </si>
   <si>
     <t>in.text</t>
@@ -343,7 +345,7 @@
     <t>{'user-agent': 'my-app/0.0.1'}</t>
   </si>
   <si>
-    <t>2017-09-28 19:40:15</t>
+    <t>2017-09-28 21:57:37</t>
   </si>
   <si>
     <t>params</t>
@@ -358,7 +360,7 @@
     <t>equal.status_code</t>
   </si>
   <si>
-    <t>qeual.ok</t>
+    <t>equal.ok</t>
   </si>
   <si>
     <t>!in.text</t>
@@ -406,12 +408,6 @@
     <t>&lt;/params&gt;</t>
   </si>
   <si>
-    <t>in.status</t>
-  </si>
-  <si>
-    <t>ok</t>
-  </si>
-  <si>
     <t>zzz</t>
   </si>
   <si>
@@ -428,55 +424,48 @@
   </si>
   <si>
     <t>AT.Login.13</t>
-  </si>
-  <si>
-    <t>n</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>y</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
+      <name val="DengXian"/>
+      <charset val="134"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="DengXian"/>
-      <family val="2"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="DengXian"/>
       <charset val="134"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="DengXian"/>
+      <charset val="134"/>
+      <family val="2"/>
       <sz val="9"/>
-      <name val="DengXian"/>
-      <family val="2"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
+        <fgColor theme="7" tint="0.7999816888943144"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -500,31 +489,28 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+  <cellXfs count="6">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="1" xfId="0">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="常规" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium7" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -790,32 +776,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView showRuler="0" tabSelected="1" topLeftCell="A12" workbookViewId="0" zoomScale="125" zoomScaleNormal="125">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="7" style="4" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="15.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5" style="4" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="38.1640625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="16" style="4" customWidth="1"/>
-    <col min="9" max="9" width="29" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.33203125" style="4" customWidth="1"/>
-    <col min="11" max="11" width="19.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="80.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="21" width="10.83203125" style="4" customWidth="1"/>
-    <col min="22" max="16384" width="10.83203125" style="4"/>
+    <col customWidth="1" max="1" min="1" style="4" width="7"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" style="4" width="14.6640625"/>
+    <col customWidth="1" max="3" min="3" style="4" width="20.33203125"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" style="4" width="15.5"/>
+    <col customWidth="1" max="5" min="5" style="4" width="11.5"/>
+    <col customWidth="1" max="6" min="6" style="4" width="14.1640625"/>
+    <col customWidth="1" max="7" min="7" style="4" width="38.1640625"/>
+    <col customWidth="1" max="8" min="8" style="4" width="16"/>
+    <col bestFit="1" customWidth="1" max="9" min="9" style="4" width="29"/>
+    <col customWidth="1" max="10" min="10" style="4" width="9.33203125"/>
+    <col bestFit="1" customWidth="1" max="11" min="11" style="4" width="19.6640625"/>
+    <col bestFit="1" customWidth="1" max="12" min="12" style="4" width="80.1640625"/>
+    <col customWidth="1" max="21" min="13" style="4" width="10.83203125"/>
+    <col customWidth="1" max="16384" min="22" style="4" width="10.83203125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="1" s="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -853,9 +843,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2" s="2" t="s">
-        <v>133</v>
+        <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>12</v>
@@ -869,23 +859,23 @@
       <c r="E2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="F2" s="3" t="n"/>
+      <c r="G2" s="3" t="n"/>
       <c r="H2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="3"/>
+      <c r="I2" s="3" t="n"/>
       <c r="J2" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="3"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L2" s="3" t="n"/>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="2" t="s">
-        <v>133</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>19</v>
@@ -899,8 +889,8 @@
       <c r="E3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="F3" s="3" t="n"/>
+      <c r="G3" s="3" t="n"/>
       <c r="H3" s="2" t="s">
         <v>16</v>
       </c>
@@ -913,14 +903,14 @@
       <c r="K3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="3"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L3" s="3" t="n"/>
+    </row>
+    <row r="4" spans="1:12">
       <c r="H4" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12">
       <c r="H5" s="4" t="s">
         <v>16</v>
       </c>
@@ -928,9 +918,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12">
       <c r="A6" s="2" t="s">
-        <v>133</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>26</v>
@@ -944,8 +934,8 @@
       <c r="E6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+      <c r="F6" s="3" t="n"/>
+      <c r="G6" s="3" t="n"/>
       <c r="H6" s="2" t="s">
         <v>16</v>
       </c>
@@ -958,9 +948,9 @@
       <c r="K6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="L6" s="3"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L6" s="3" t="n"/>
+    </row>
+    <row r="7" spans="1:12">
       <c r="D7" s="4" t="s">
         <v>30</v>
       </c>
@@ -977,7 +967,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12">
       <c r="D8" s="4" t="s">
         <v>35</v>
       </c>
@@ -988,7 +978,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12">
       <c r="D9" s="4" t="s">
         <v>38</v>
       </c>
@@ -1002,9 +992,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12">
       <c r="A10" s="2" t="s">
-        <v>133</v>
+        <v>11</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>41</v>
@@ -1018,8 +1008,8 @@
       <c r="E10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
+      <c r="F10" s="3" t="n"/>
+      <c r="G10" s="3" t="n"/>
       <c r="H10" s="2" t="s">
         <v>16</v>
       </c>
@@ -1032,9 +1022,9 @@
       <c r="K10" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="L10" s="3"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L10" s="3" t="n"/>
+    </row>
+    <row r="11" spans="1:12">
       <c r="D11" s="4" t="s">
         <v>44</v>
       </c>
@@ -1051,15 +1041,15 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12">
       <c r="H12" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="I12" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I12" s="4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="F13" s="4" t="s">
         <v>31</v>
       </c>
@@ -1070,89 +1060,89 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12">
       <c r="A14" s="2" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
+      <c r="F14" s="3" t="n"/>
+      <c r="G14" s="3" t="n"/>
       <c r="H14" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="D15" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>33</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="D16" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>33</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="D17" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="D18" s="4" t="s">
         <v>40</v>
       </c>
@@ -1160,231 +1150,231 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12">
       <c r="A19" s="2" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
+      <c r="F19" s="3" t="n"/>
+      <c r="G19" s="3" t="n"/>
       <c r="H19" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J19" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="L19" s="3"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="L19" s="3" t="n"/>
+    </row>
+    <row r="20" spans="1:12">
       <c r="D20" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="I20" s="4">
+        <v>64</v>
+      </c>
+      <c r="I20" s="4" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12">
       <c r="D21" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H21" s="4" t="s">
         <v>33</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
       <c r="D22" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H22" s="4" t="s">
         <v>33</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
       <c r="D23" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24" s="2" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D24" s="3"/>
+        <v>77</v>
+      </c>
+      <c r="D24" s="3" t="n"/>
       <c r="E24" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
+        <v>78</v>
+      </c>
+      <c r="F24" s="3" t="n"/>
+      <c r="G24" s="3" t="n"/>
       <c r="H24" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J24" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="L24" s="3"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+      <c r="L24" s="3" t="n"/>
+    </row>
+    <row r="25" spans="1:12">
       <c r="H25" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
       <c r="A26" s="2" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D26" s="3"/>
+        <v>85</v>
+      </c>
+      <c r="D26" s="3" t="n"/>
       <c r="E26" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
+        <v>78</v>
+      </c>
+      <c r="F26" s="3" t="n"/>
+      <c r="G26" s="3" t="n"/>
       <c r="H26" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="J26" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="L26" s="3"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+      <c r="L26" s="3" t="n"/>
+    </row>
+    <row r="27" spans="1:12">
       <c r="H27" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
       <c r="A28" s="2" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
+      <c r="C28" s="3" t="n"/>
+      <c r="D28" s="3" t="n"/>
+      <c r="E28" s="3" t="n"/>
       <c r="F28" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>33</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+      <c r="J28" s="3" t="n"/>
+      <c r="K28" s="3" t="n"/>
+      <c r="L28" s="3" t="n"/>
+    </row>
+    <row r="29" spans="1:12">
       <c r="H29" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I29" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="H30" s="4" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="H30" s="4" t="s">
-        <v>73</v>
-      </c>
       <c r="I30" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
       <c r="H31" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
       <c r="H32" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
       <c r="A33" s="2" t="s">
-        <v>91</v>
+        <v>11</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>92</v>
@@ -1392,12 +1382,12 @@
       <c r="C33" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D33" s="3"/>
+      <c r="D33" s="3" t="n"/>
       <c r="E33" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
+      <c r="F33" s="3" t="n"/>
+      <c r="G33" s="3" t="n"/>
       <c r="H33" s="2" t="s">
         <v>95</v>
       </c>
@@ -1410,9 +1400,9 @@
       <c r="K33" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="L33" s="3"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L33" s="3" t="n"/>
+    </row>
+    <row r="34" spans="1:12">
       <c r="H34" s="4" t="s">
         <v>98</v>
       </c>
@@ -1420,9 +1410,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12">
       <c r="A35" s="2" t="s">
-        <v>91</v>
+        <v>11</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>100</v>
@@ -1430,7 +1420,7 @@
       <c r="C35" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D35" s="3"/>
+      <c r="D35" s="3" t="n"/>
       <c r="E35" s="2" t="s">
         <v>94</v>
       </c>
@@ -1440,17 +1430,17 @@
       <c r="G35" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
+      <c r="H35" s="3" t="n"/>
+      <c r="I35" s="3" t="n"/>
       <c r="J35" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K35" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="L35" s="3"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L35" s="3" t="n"/>
+    </row>
+    <row r="36" spans="1:12">
       <c r="F36" s="4" t="s">
         <v>104</v>
       </c>
@@ -1458,26 +1448,26 @@
         <v>105</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12">
       <c r="F37" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="G37" s="4">
+      <c r="G37" s="4" t="n">
         <v>2</v>
       </c>
       <c r="H37" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12">
       <c r="H38" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="I38" s="4">
+      <c r="I38" s="4" t="n">
         <v>200</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12">
       <c r="H39" s="4" t="s">
         <v>108</v>
       </c>
@@ -1485,7 +1475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12">
       <c r="H40" s="4" t="s">
         <v>109</v>
       </c>
@@ -1493,7 +1483,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12">
       <c r="H41" s="4" t="s">
         <v>111</v>
       </c>
@@ -1501,9 +1491,9 @@
         <v>112</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12">
       <c r="A42" s="2" t="s">
-        <v>132</v>
+        <v>11</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>113</v>
@@ -1511,21 +1501,25 @@
       <c r="C42" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D42" s="3"/>
+      <c r="D42" s="3" t="n"/>
       <c r="E42" s="2" t="s">
         <v>94</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="G42" s="2"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
-      <c r="K42" s="3"/>
-      <c r="L42" s="3"/>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G42" s="2" t="n"/>
+      <c r="H42" s="3" t="n"/>
+      <c r="I42" s="3" t="n"/>
+      <c r="J42" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K42" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="L42" s="3" t="s"/>
+    </row>
+    <row r="43" spans="1:12">
       <c r="F43" s="4" t="s">
         <v>115</v>
       </c>
@@ -1533,17 +1527,17 @@
         <v>116</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12">
       <c r="F44" s="4" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12">
       <c r="F45" s="4" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12">
       <c r="F46" s="4" t="s">
         <v>119</v>
       </c>
@@ -1551,7 +1545,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12">
       <c r="F47" s="4" t="s">
         <v>121</v>
       </c>
@@ -1559,23 +1553,23 @@
         <v>122</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12">
       <c r="F48" s="4" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="49" spans="6:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12">
       <c r="F49" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="G49" s="4">
+      <c r="G49" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="H49" s="4" t="s">
+      <c r="H49" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="50" spans="6:9" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row customHeight="1" ht="19" r="50" spans="1:12">
       <c r="H50" s="4" t="s">
         <v>109</v>
       </c>
@@ -1583,52 +1577,49 @@
         <v>110</v>
       </c>
     </row>
-    <row r="51" spans="6:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12">
       <c r="H51" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="I51" s="4" t="s">
         <v>124</v>
-      </c>
-      <c r="I51" s="4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="52" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="H52" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="I52" s="4" t="s">
-        <v>126</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:K41"/>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView showRuler="0" zoomScale="125" zoomScaleNormal="125" workbookViewId="0"/>
+    <sheetView showRuler="0" workbookViewId="0" zoomScale="125" zoomScaleNormal="125">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="12.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.6640625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="8.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="31.83203125" style="4" customWidth="1"/>
-    <col min="13" max="20" width="10.83203125" style="4" customWidth="1"/>
-    <col min="21" max="16384" width="10.83203125" style="4"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="4" width="8.1640625"/>
+    <col bestFit="1" customWidth="1" max="4" min="2" style="4" width="12.1640625"/>
+    <col bestFit="1" customWidth="1" max="5" min="5" style="4" width="8.1640625"/>
+    <col bestFit="1" customWidth="1" max="6" min="6" style="4" width="12.83203125"/>
+    <col bestFit="1" customWidth="1" max="7" min="7" style="4" width="28.1640625"/>
+    <col bestFit="1" customWidth="1" max="8" min="8" style="4" width="12.83203125"/>
+    <col customWidth="1" max="9" min="9" style="4" width="30.6640625"/>
+    <col bestFit="1" customWidth="1" max="10" min="10" style="4" width="8.1640625"/>
+    <col bestFit="1" customWidth="1" max="11" min="11" style="4" width="19.6640625"/>
+    <col customWidth="1" max="12" min="12" style="4" width="31.83203125"/>
+    <col customWidth="1" max="20" min="13" style="4" width="10.83203125"/>
+    <col customWidth="1" max="16384" min="21" style="4" width="10.83203125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="1" s="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1666,88 +1657,88 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2" s="3" t="n"/>
+      <c r="E2" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="F2" s="3" t="n"/>
+      <c r="G2" s="3" t="n"/>
       <c r="H2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I2" s="3" t="n"/>
+      <c r="J2" s="3" t="n"/>
+      <c r="K2" s="3" t="n"/>
+      <c r="L2" s="3" t="n"/>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="2" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D3" s="3"/>
+        <v>126</v>
+      </c>
+      <c r="D3" s="3" t="n"/>
       <c r="E3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="F3" s="3" t="n"/>
+      <c r="G3" s="3" t="n"/>
       <c r="H3" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J3" s="3" t="n"/>
+      <c r="K3" s="3" t="n"/>
+      <c r="L3" s="3" t="n"/>
+    </row>
+    <row r="4" spans="1:12">
       <c r="H4" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D5" s="3"/>
+        <v>126</v>
+      </c>
+      <c r="D5" s="3" t="n"/>
       <c r="E5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
+      <c r="F5" s="3" t="n"/>
+      <c r="G5" s="3" t="n"/>
       <c r="H5" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J5" s="3" t="n"/>
+      <c r="K5" s="3" t="n"/>
+      <c r="L5" s="3" t="n"/>
+    </row>
+    <row r="6" spans="1:12">
       <c r="F6" s="4" t="s">
         <v>31</v>
       </c>
@@ -1761,7 +1752,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12">
       <c r="F7" s="4" t="s">
         <v>31</v>
       </c>
@@ -1772,14 +1763,13 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12">
       <c r="H8" s="4" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:K8"/>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Rename locate to locator.
</commit_message>
<xml_diff>
--- a/Cases/Cases1.xlsx
+++ b/Cases/Cases1.xlsx
@@ -1,40 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28502"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jia/Dropbox/v2test/Cases/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17620"/>
   </bookViews>
   <sheets>
-    <sheet name="Tests1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Tests2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Tests1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tests2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tests1!$A$1:$K$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tests2!$A$1:$K$8</definedName>
   </definedNames>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="132">
   <si>
     <t>Run</t>
   </si>
@@ -424,48 +422,55 @@
   </si>
   <si>
     <t>AT.Login.13</t>
+  </si>
+  <si>
+    <t>Action</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Locator/Encapsulator</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="DengXian"/>
+      <family val="2"/>
       <charset val="134"/>
-      <family val="2"/>
-      <color theme="1"/>
-      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="DengXian"/>
       <charset val="134"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="9"/>
       <name val="DengXian"/>
+      <family val="2"/>
       <charset val="134"/>
-      <family val="2"/>
-      <sz val="9"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.7999816888943144"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -489,28 +494,34 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="1" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="常规" xfId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium7" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -776,36 +787,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView showRuler="0" tabSelected="1" topLeftCell="A12" workbookViewId="0" zoomScale="125" zoomScaleNormal="125">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="4" width="7"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" style="4" width="14.6640625"/>
-    <col customWidth="1" max="3" min="3" style="4" width="20.33203125"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" style="4" width="15.5"/>
-    <col customWidth="1" max="5" min="5" style="4" width="11.5"/>
-    <col customWidth="1" max="6" min="6" style="4" width="14.1640625"/>
-    <col customWidth="1" max="7" min="7" style="4" width="38.1640625"/>
-    <col customWidth="1" max="8" min="8" style="4" width="16"/>
-    <col bestFit="1" customWidth="1" max="9" min="9" style="4" width="29"/>
-    <col customWidth="1" max="10" min="10" style="4" width="9.33203125"/>
-    <col bestFit="1" customWidth="1" max="11" min="11" style="4" width="19.6640625"/>
-    <col bestFit="1" customWidth="1" max="12" min="12" style="4" width="80.1640625"/>
-    <col customWidth="1" max="21" min="13" style="4" width="10.83203125"/>
-    <col customWidth="1" max="16384" min="22" style="4" width="10.83203125"/>
+    <col min="1" max="1" width="7" style="4" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5" style="4" customWidth="1"/>
+    <col min="6" max="6" width="14.5" style="4" customWidth="1"/>
+    <col min="7" max="7" width="38.1640625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="16" style="4" customWidth="1"/>
+    <col min="9" max="9" width="29" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="19.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="80.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="22" width="10.83203125" style="4" customWidth="1"/>
+    <col min="23" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:12">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -822,13 +829,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>131</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>130</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>6</v>
@@ -843,7 +850,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -859,21 +866,21 @@
       <c r="E2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="3" t="n"/>
-      <c r="G2" s="3" t="n"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
       <c r="H2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="3" t="n"/>
+      <c r="I2" s="3"/>
       <c r="J2" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="3" t="n"/>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="L2" s="3"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -889,8 +896,8 @@
       <c r="E3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="3" t="n"/>
-      <c r="G3" s="3" t="n"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
       <c r="H3" s="2" t="s">
         <v>16</v>
       </c>
@@ -903,14 +910,14 @@
       <c r="K3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="3" t="n"/>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="L3" s="3"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H4" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H5" s="4" t="s">
         <v>16</v>
       </c>
@@ -918,7 +925,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -934,8 +941,8 @@
       <c r="E6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="3" t="n"/>
-      <c r="G6" s="3" t="n"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
       <c r="H6" s="2" t="s">
         <v>16</v>
       </c>
@@ -948,9 +955,9 @@
       <c r="K6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="L6" s="3" t="n"/>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="L6" s="3"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D7" s="4" t="s">
         <v>30</v>
       </c>
@@ -967,7 +974,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D8" s="4" t="s">
         <v>35</v>
       </c>
@@ -978,7 +985,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D9" s="4" t="s">
         <v>38</v>
       </c>
@@ -992,7 +999,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -1008,8 +1015,8 @@
       <c r="E10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="3" t="n"/>
-      <c r="G10" s="3" t="n"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
       <c r="H10" s="2" t="s">
         <v>16</v>
       </c>
@@ -1022,9 +1029,9 @@
       <c r="K10" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="L10" s="3" t="n"/>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="L10" s="3"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D11" s="4" t="s">
         <v>44</v>
       </c>
@@ -1041,15 +1048,15 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H12" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="I12" s="4" t="n">
+      <c r="I12" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F13" s="4" t="s">
         <v>31</v>
       </c>
@@ -1060,7 +1067,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>47</v>
       </c>
@@ -1076,8 +1083,8 @@
       <c r="E14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="3" t="n"/>
-      <c r="G14" s="3" t="n"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
       <c r="H14" s="2" t="s">
         <v>16</v>
       </c>
@@ -1094,7 +1101,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D15" s="4" t="s">
         <v>55</v>
       </c>
@@ -1111,7 +1118,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D16" s="4" t="s">
         <v>59</v>
       </c>
@@ -1128,7 +1135,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D17" s="4" t="s">
         <v>62</v>
       </c>
@@ -1142,7 +1149,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D18" s="4" t="s">
         <v>40</v>
       </c>
@@ -1150,7 +1157,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>47</v>
       </c>
@@ -1166,8 +1173,8 @@
       <c r="E19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="3" t="n"/>
-      <c r="G19" s="3" t="n"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
       <c r="H19" s="2" t="s">
         <v>16</v>
       </c>
@@ -1180,9 +1187,9 @@
       <c r="K19" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="L19" s="3" t="n"/>
-    </row>
-    <row r="20" spans="1:12">
+      <c r="L19" s="3"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D20" s="4" t="s">
         <v>69</v>
       </c>
@@ -1195,11 +1202,11 @@
       <c r="H20" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="I20" s="4" t="n">
+      <c r="I20" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D21" s="4" t="s">
         <v>70</v>
       </c>
@@ -1210,7 +1217,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D22" s="4" t="s">
         <v>72</v>
       </c>
@@ -1227,7 +1234,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D23" s="4" t="s">
         <v>73</v>
       </c>
@@ -1238,7 +1245,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>47</v>
       </c>
@@ -1248,12 +1255,12 @@
       <c r="C24" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D24" s="3" t="n"/>
+      <c r="D24" s="3"/>
       <c r="E24" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F24" s="3" t="n"/>
-      <c r="G24" s="3" t="n"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
       <c r="H24" s="2" t="s">
         <v>79</v>
       </c>
@@ -1266,9 +1273,9 @@
       <c r="K24" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="L24" s="3" t="n"/>
-    </row>
-    <row r="25" spans="1:12">
+      <c r="L24" s="3"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H25" s="4" t="s">
         <v>82</v>
       </c>
@@ -1276,7 +1283,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>47</v>
       </c>
@@ -1286,12 +1293,12 @@
       <c r="C26" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D26" s="3" t="n"/>
+      <c r="D26" s="3"/>
       <c r="E26" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F26" s="3" t="n"/>
-      <c r="G26" s="3" t="n"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
       <c r="H26" s="2" t="s">
         <v>86</v>
       </c>
@@ -1304,9 +1311,9 @@
       <c r="K26" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="L26" s="3" t="n"/>
-    </row>
-    <row r="27" spans="1:12">
+      <c r="L26" s="3"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H27" s="4" t="s">
         <v>82</v>
       </c>
@@ -1314,16 +1321,16 @@
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C28" s="3" t="n"/>
-      <c r="D28" s="3" t="n"/>
-      <c r="E28" s="3" t="n"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
       <c r="F28" s="2" t="s">
         <v>56</v>
       </c>
@@ -1336,11 +1343,11 @@
       <c r="I28" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="J28" s="3" t="n"/>
-      <c r="K28" s="3" t="n"/>
-      <c r="L28" s="3" t="n"/>
-    </row>
-    <row r="29" spans="1:12">
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H29" s="4" t="s">
         <v>74</v>
       </c>
@@ -1348,7 +1355,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H30" s="4" t="s">
         <v>74</v>
       </c>
@@ -1356,7 +1363,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H31" s="4" t="s">
         <v>90</v>
       </c>
@@ -1364,7 +1371,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H32" s="4" t="s">
         <v>82</v>
       </c>
@@ -1372,7 +1379,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>11</v>
       </c>
@@ -1382,12 +1389,12 @@
       <c r="C33" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D33" s="3" t="n"/>
+      <c r="D33" s="3"/>
       <c r="E33" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="F33" s="3" t="n"/>
-      <c r="G33" s="3" t="n"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
       <c r="H33" s="2" t="s">
         <v>95</v>
       </c>
@@ -1400,9 +1407,9 @@
       <c r="K33" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="L33" s="3" t="n"/>
-    </row>
-    <row r="34" spans="1:12">
+      <c r="L33" s="3"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H34" s="4" t="s">
         <v>98</v>
       </c>
@@ -1410,7 +1417,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>11</v>
       </c>
@@ -1420,7 +1427,7 @@
       <c r="C35" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D35" s="3" t="n"/>
+      <c r="D35" s="3"/>
       <c r="E35" s="2" t="s">
         <v>94</v>
       </c>
@@ -1430,17 +1437,17 @@
       <c r="G35" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="H35" s="3" t="n"/>
-      <c r="I35" s="3" t="n"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
       <c r="J35" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K35" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="L35" s="3" t="n"/>
-    </row>
-    <row r="36" spans="1:12">
+      <c r="L35" s="3"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F36" s="4" t="s">
         <v>104</v>
       </c>
@@ -1448,26 +1455,26 @@
         <v>105</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F37" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="G37" s="4" t="n">
+      <c r="G37" s="4">
         <v>2</v>
       </c>
       <c r="H37" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H38" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="I38" s="4" t="n">
+      <c r="I38" s="4">
         <v>200</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H39" s="4" t="s">
         <v>108</v>
       </c>
@@ -1475,7 +1482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H40" s="4" t="s">
         <v>109</v>
       </c>
@@ -1483,7 +1490,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H41" s="4" t="s">
         <v>111</v>
       </c>
@@ -1491,7 +1498,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>11</v>
       </c>
@@ -1501,25 +1508,25 @@
       <c r="C42" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D42" s="3" t="n"/>
+      <c r="D42" s="3"/>
       <c r="E42" s="2" t="s">
         <v>94</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="G42" s="2" t="n"/>
-      <c r="H42" s="3" t="n"/>
-      <c r="I42" s="3" t="n"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
       <c r="J42" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K42" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="L42" s="3" t="s"/>
-    </row>
-    <row r="43" spans="1:12">
+      <c r="L42" s="3"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F43" s="4" t="s">
         <v>115</v>
       </c>
@@ -1527,17 +1534,17 @@
         <v>116</v>
       </c>
     </row>
-    <row r="44" spans="1:12">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F44" s="4" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="45" spans="1:12">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F45" s="4" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="46" spans="1:12">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F46" s="4" t="s">
         <v>119</v>
       </c>
@@ -1545,7 +1552,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="47" spans="1:12">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F47" s="4" t="s">
         <v>121</v>
       </c>
@@ -1553,23 +1560,23 @@
         <v>122</v>
       </c>
     </row>
-    <row r="48" spans="1:12">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F48" s="4" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="49" spans="1:12">
+    <row r="49" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F49" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="G49" s="4" t="n">
+      <c r="G49" s="4">
         <v>5</v>
       </c>
       <c r="H49" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row customHeight="1" ht="19" r="50" spans="1:12">
+    <row r="50" spans="6:9" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H50" s="4" t="s">
         <v>109</v>
       </c>
@@ -1577,7 +1584,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="51" spans="1:12">
+    <row r="51" spans="6:9" x14ac:dyDescent="0.2">
       <c r="H51" s="4" t="s">
         <v>111</v>
       </c>
@@ -1587,39 +1594,34 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:K41"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" zoomScale="125" zoomScaleNormal="125">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView showRuler="0" zoomScale="125" zoomScaleNormal="125" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="4" width="8.1640625"/>
-    <col bestFit="1" customWidth="1" max="4" min="2" style="4" width="12.1640625"/>
-    <col bestFit="1" customWidth="1" max="5" min="5" style="4" width="8.1640625"/>
-    <col bestFit="1" customWidth="1" max="6" min="6" style="4" width="12.83203125"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" style="4" width="28.1640625"/>
-    <col bestFit="1" customWidth="1" max="8" min="8" style="4" width="12.83203125"/>
-    <col customWidth="1" max="9" min="9" style="4" width="30.6640625"/>
-    <col bestFit="1" customWidth="1" max="10" min="10" style="4" width="8.1640625"/>
-    <col bestFit="1" customWidth="1" max="11" min="11" style="4" width="19.6640625"/>
-    <col customWidth="1" max="12" min="12" style="4" width="31.83203125"/>
-    <col customWidth="1" max="20" min="13" style="4" width="10.83203125"/>
-    <col customWidth="1" max="16384" min="21" style="4" width="10.83203125"/>
+    <col min="1" max="1" width="8.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="12.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.6640625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="8.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31.83203125" style="4" customWidth="1"/>
+    <col min="13" max="21" width="10.83203125" style="4" customWidth="1"/>
+    <col min="22" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:12">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1657,7 +1659,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>47</v>
       </c>
@@ -1667,21 +1669,21 @@
       <c r="C2" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D2" s="3" t="n"/>
+      <c r="D2" s="3"/>
       <c r="E2" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="F2" s="3" t="n"/>
-      <c r="G2" s="3" t="n"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
       <c r="H2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="3" t="n"/>
-      <c r="J2" s="3" t="n"/>
-      <c r="K2" s="3" t="n"/>
-      <c r="L2" s="3" t="n"/>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>47</v>
       </c>
@@ -1691,28 +1693,28 @@
       <c r="C3" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D3" s="3" t="n"/>
+      <c r="D3" s="3"/>
       <c r="E3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="3" t="n"/>
-      <c r="G3" s="3" t="n"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
       <c r="H3" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="3" t="n"/>
-      <c r="K3" s="3" t="n"/>
-      <c r="L3" s="3" t="n"/>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H4" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>47</v>
       </c>
@@ -1722,23 +1724,23 @@
       <c r="C5" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D5" s="3" t="n"/>
+      <c r="D5" s="3"/>
       <c r="E5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="3" t="n"/>
-      <c r="G5" s="3" t="n"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
       <c r="H5" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J5" s="3" t="n"/>
-      <c r="K5" s="3" t="n"/>
-      <c r="L5" s="3" t="n"/>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F6" s="4" t="s">
         <v>31</v>
       </c>
@@ -1752,7 +1754,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F7" s="4" t="s">
         <v>31</v>
       </c>
@@ -1763,13 +1765,14 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H8" s="4" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:K8"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add usage for framework.
</commit_message>
<xml_diff>
--- a/Cases/Cases1.xlsx
+++ b/Cases/Cases1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17620"/>
+    <workbookView xWindow="31560" yWindow="1460" windowWidth="28800" windowHeight="17620"/>
   </bookViews>
   <sheets>
     <sheet name="Tests1" sheetId="1" r:id="rId1"/>
@@ -791,7 +791,7 @@
   <dimension ref="A1:L51"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1147,6 +1147,9 @@
       </c>
       <c r="H17" s="4" t="s">
         <v>64</v>
+      </c>
+      <c r="I17" s="4">
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">

</xml_diff>